<commit_message>
Data Structure_Singly Sorted Linked List
:(
</commit_message>
<xml_diff>
--- a/source/repos/Container_Prac/C++ STL.xlsx
+++ b/source/repos/Container_Prac/C++ STL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KoMoGoon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KoMoGoon\Documents\GitHub\Mukho\source\repos\Container_Prac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1666BA1E-D015-455B-9196-C89C4BFDA1D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED48956-6EAE-4EE4-B181-80DD6CF764C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="1380" windowWidth="21600" windowHeight="11385" xr2:uid="{9FEDEF59-FFD3-4DC8-AA8B-E305926CFFFD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9FEDEF59-FFD3-4DC8-AA8B-E305926CFFFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="99">
   <si>
-    <t>C++ Standart Template Library</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>함수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -427,6 +423,10 @@
   </si>
   <si>
     <t>list와 list 사이에서 원소 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C++ Standard Template Library</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -834,6 +834,90 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -852,72 +936,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -941,24 +959,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1276,9 +1276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6824296-B392-4AE0-9D90-9CDCF2B9F274}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1295,764 +1293,764 @@
   <sheetData>
     <row r="1" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="34"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="39"/>
+      <c r="C4" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="39"/>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="41"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="41"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="42"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="32" t="s">
+      <c r="C10" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="18"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="18"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="18"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="16"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="18"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="18"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="16"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="18"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="24"/>
+      <c r="C23" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="24"/>
+      <c r="C25" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="16"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="24"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="18"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="24"/>
+      <c r="C27" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="16"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="24"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="18"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="24"/>
+      <c r="C29" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="16"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="24"/>
+      <c r="C30" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="18"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="24"/>
+      <c r="C31" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="16"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="24"/>
+      <c r="C32" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="18"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="24"/>
+      <c r="C33" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="16"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="24"/>
+      <c r="C34" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="18"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="24"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="16"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="24"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="18"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="24"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="16"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="18"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="35"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="36"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="15"/>
-    </row>
-    <row r="10" spans="1:8" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="22"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="24"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="22"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="24"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="22"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="24"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" s="22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="24"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="22"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="38"/>
-      <c r="C22" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="24"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H23" s="22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="38"/>
-      <c r="C24" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="H24" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="22"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="24"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="22"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="E28" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="24"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="22"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D30" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="24"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="22"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" s="38"/>
-      <c r="C32" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E32" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="24"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="22"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="24"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B35" s="38"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="22"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" s="38"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="24"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B37" s="38"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="22"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B38" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23" t="s">
+      <c r="C39" s="10"/>
+      <c r="D39" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="24"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="7" t="s">
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="16"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="40" t="s">
+      <c r="B40" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16" t="s">
+      <c r="C40" s="17"/>
+      <c r="D40" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="22"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="20" t="s">
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="18"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="40" t="s">
+      <c r="B41" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23" t="s">
+      <c r="C41" s="10"/>
+      <c r="D41" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E40" s="23"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="23"/>
-      <c r="H40" s="24"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="16"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B41" s="41" t="s">
-        <v>94</v>
-      </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="22"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="20" t="s">
+      <c r="G42" s="17"/>
+      <c r="H42" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="41" t="s">
+      <c r="B43" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23" t="s">
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G42" s="23"/>
-      <c r="H42" s="24" t="s">
+      <c r="G43" s="10" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
+      <c r="H43" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="41" t="s">
-        <v>96</v>
-      </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16" t="s">
+      <c r="B44" s="28"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="G43" s="16" t="s">
+      <c r="G44" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="H43" s="22" t="s">
+      <c r="H44" s="20" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="B44" s="42"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="G44" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="H44" s="26" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>